<commit_message>
Ajout du diagramme de classe
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5878B64-F1FF-41A1-B0ED-8AC26686D2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7D6BE6-5663-40AE-8F52-D3D58EBE06E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -125,6 +125,50 @@
   </si>
   <si>
     <t>Amélioration du style pour le dossier de projet et le journal de travai</t>
+  </si>
+  <si>
+    <t>Écriture de l'email pour l'envoi de la planification initiale</t>
+  </si>
+  <si>
+    <t>Création du diagramme de classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je me sens confient pour la suite du projet </t>
+  </si>
+  <si>
+    <t>Création des milestones, des tags et du projet KanBan sur GitHub</t>
+  </si>
+  <si>
+    <t>Création des tâches sur GitHub</t>
+  </si>
+  <si>
+    <t>Réalisation du diagramme de classes</t>
+  </si>
+  <si>
+    <t>Validation du diagramme de classes</t>
+  </si>
+  <si>
+    <t>Validation faite avec Monsieur Viret</t>
+  </si>
+  <si>
+    <t>Rectification du diagramme de classes</t>
+  </si>
+  <si>
+    <t>Écriture de l'analyse du diagramme de classes</t>
+  </si>
+  <si>
+    <t>Écriture de la planification initiale</t>
+  </si>
+  <si>
+    <t>Création du diagramme de flux la gestion du mouvement des pièces</t>
+  </si>
+  <si>
+    <t>Guide pour les relations:
+https://cpnv-es-ngy.gitbook.io/uml-backlog/class-diagram/standards/les-relations</t>
+  </si>
+  <si>
+    <t>Comment utiliser astah:
+https://astah.net/support/astah-pro/user-guide/class-diagrams/</t>
   </si>
 </sst>
 </file>
@@ -493,8 +537,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val -104509"/>
-                        <a:gd name="adj2" fmla="val 158466"/>
+                        <a:gd name="adj1" fmla="val -182261"/>
+                        <a:gd name="adj2" fmla="val -43804"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -581,8 +625,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val -107387"/>
-                        <a:gd name="adj2" fmla="val -2230"/>
+                        <a:gd name="adj1" fmla="val 57122"/>
+                        <a:gd name="adj2" fmla="val -204500"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -600,8 +644,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.22222222222222221"/>
-                  <c:y val="-5.0925925925925923E-2"/>
+                  <c:x val="-3.6111111111111122E-2"/>
+                  <c:y val="-4.6296296296296294E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -669,8 +713,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val -102116"/>
-                        <a:gd name="adj2" fmla="val -148637"/>
+                        <a:gd name="adj1" fmla="val 134499"/>
+                        <a:gd name="adj2" fmla="val -23706"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -688,8 +732,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.8333333333333362E-2"/>
-                  <c:y val="1.3888888888888805E-2"/>
+                  <c:x val="-7.5000000000000025E-2"/>
+                  <c:y val="1.3888888888888846E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -757,8 +801,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 199659"/>
-                        <a:gd name="adj2" fmla="val -20773"/>
+                        <a:gd name="adj1" fmla="val 253308"/>
+                        <a:gd name="adj2" fmla="val 74413"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -946,19 +990,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.22972972972972994</c:v>
+                  <c:v>0.57432432432432456</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.49999999999999989</c:v>
+                  <c:v>0.27027027027027017</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27027027027027017</c:v>
+                  <c:v>0.15540540540540529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1972,8 +2016,8 @@
   </sheetPr>
   <dimension ref="B3:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1985,7 +2029,7 @@
     <col min="6" max="6" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="61.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="55.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2225,102 +2269,234 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="8">
+        <v>45412</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.69444444444444453</v>
+      </c>
       <c r="E13" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.7777777777777901E-2</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+      <c r="B14" s="8">
+        <v>45412</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="E14" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="B15" s="8">
+        <v>45414</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="E15" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+      <c r="B16" s="8">
+        <v>45414</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.4513888888888889</v>
+      </c>
       <c r="E16" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+    <row r="17" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>45414</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E17" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>5.9027777777777735E-2</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
+    <row r="18" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>45414</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.59375</v>
+      </c>
       <c r="E18" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="B19" s="8">
+        <v>45414</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.59375</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="E19" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+      <c r="B20" s="8">
+        <v>45414</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="E20" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+      <c r="B21" s="8">
+        <v>45414</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.64930555555555558</v>
+      </c>
       <c r="E21" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
+    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="8">
+        <v>45414</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.67013888888888884</v>
+      </c>
       <c r="E22" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="J22" s="1"/>
     </row>
@@ -2653,10 +2829,14 @@
       <c r="J80" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I17" r:id="rId1" display="https://astah.net/support/astah-pro/user-guide/class-diagrams/" xr:uid="{7C32A445-90EE-437F-9496-B44EF63F2338}"/>
+    <hyperlink ref="I18" r:id="rId2" display="https://cpnv-es-ngy.gitbook.io/uml-backlog/class-diagram/standards/les-relations" xr:uid="{91F5105D-276F-4EB5-A9C4-C4F8D89CE4EA}"/>
+  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="landscape" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2665,8 +2845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E5A45F-AFC1-4C75-BD5B-45FB52BA7D0E}">
   <dimension ref="C3:I80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2706,7 +2886,7 @@
       </c>
       <c r="D4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!D$3, Tableau1[Durée])</f>
-        <v>5.902777777777779E-2</v>
+        <v>0.29513888888888878</v>
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
@@ -2714,7 +2894,7 @@
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>0.1284722222222221</v>
+        <v>0.13888888888888873</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -2722,11 +2902,11 @@
       </c>
       <c r="H4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!H$3, Tableau1[Durée])</f>
-        <v>6.9444444444444364E-2</v>
+        <v>7.9861111111110994E-2</v>
       </c>
       <c r="I4" s="4">
         <f>SUM(D4:H4)</f>
-        <v>0.25694444444444425</v>
+        <v>0.51388888888888851</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -2735,7 +2915,7 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.22972972972972994</v>
+        <v>0.57432432432432456</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
@@ -2743,7 +2923,7 @@
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.49999999999999989</v>
+        <v>0.27027027027027017</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -2751,7 +2931,7 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>0.27027027027027017</v>
+        <v>0.15540540540540529</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>

</xml_diff>

<commit_message>
Ajout des diagrammes de flux
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7D6BE6-5663-40AE-8F52-D3D58EBE06E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07330A53-5838-491F-A8A7-7EF4151C78A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -155,12 +155,6 @@
   </si>
   <si>
     <t>Écriture de l'analyse du diagramme de classes</t>
-  </si>
-  <si>
-    <t>Écriture de la planification initiale</t>
-  </si>
-  <si>
-    <t>Création du diagramme de flux la gestion du mouvement des pièces</t>
   </si>
   <si>
     <t>Guide pour les relations:
@@ -169,6 +163,45 @@
   <si>
     <t>Comment utiliser astah:
 https://astah.net/support/astah-pro/user-guide/class-diagrams/</t>
+  </si>
+  <si>
+    <t>Création du diagramme de flux de la gestion du mouvement des pièces</t>
+  </si>
+  <si>
+    <t>Création du diagramme de flux de la condition de fin de partie</t>
+  </si>
+  <si>
+    <t>https://support.microsoft.com/fr-fr/topic/cr%C3%A9er-un-diagramme-de-flux-simple-dans-visio-e207d975-4a51-4bfa-a356-eeec314bd276</t>
+  </si>
+  <si>
+    <t>Création du diagramme de flux de la gestion des mouvements spéciaux</t>
+  </si>
+  <si>
+    <t>Journal de travail - TPI Jeu d'échec sur Unity</t>
+  </si>
+  <si>
+    <t>Création du diagramme de flux pour la gestion du tour des joueurs</t>
+  </si>
+  <si>
+    <t>Création du diagramme de flux pour la gestion du fichier récapitulatif</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Algebraic_notation_(chess)</t>
+  </si>
+  <si>
+    <t>Modification des projets sur GitHub</t>
+  </si>
+  <si>
+    <t>Changement de un projet pour le GitHub à un projet pour chaque sprint du GitHub</t>
+  </si>
+  <si>
+    <t>Écriture de la planification initiale dans le dossier de projet</t>
+  </si>
+  <si>
+    <t>Écriture des diagrammes de flux dans le dossier de projet</t>
+  </si>
+  <si>
+    <t>Création des maquettes pour les menus</t>
   </si>
 </sst>
 </file>
@@ -178,7 +211,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,16 +227,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -211,12 +258,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -237,6 +321,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -990,19 +1083,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.57432432432432456</c:v>
+                  <c:v>-0.75510204081632981</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27027027027027017</c:v>
+                  <c:v>1.1836734693877577</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15540540540540529</c:v>
+                  <c:v>0.57142857142857195</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2014,10 +2107,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:J80"/>
+  <dimension ref="B1:J80"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,6 +2126,19 @@
     <col min="10" max="10" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12"/>
+    </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>0</v>
@@ -2283,10 +2389,10 @@
         <v>2.7777777777777901E-2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -2380,7 +2486,7 @@
         <v>31</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J17" s="1"/>
     </row>
@@ -2405,7 +2511,7 @@
         <v>35</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J18" s="1"/>
     </row>
@@ -2478,7 +2584,7 @@
       </c>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
         <v>45414</v>
       </c>
@@ -2496,77 +2602,168 @@
         <v>3</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
+      <c r="B23" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.3611111111111111</v>
+      </c>
       <c r="E23" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
+    <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0.37847222222222227</v>
+      </c>
       <c r="E24" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
+      <c r="B25" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="E25" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
+    <row r="26" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0.42708333333333331</v>
+      </c>
       <c r="E26" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
+    <row r="27" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0.44444444444444442</v>
+      </c>
       <c r="E27" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>1.7361111111111105E-2</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
+      <c r="B28" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="E28" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>3.4722222222222265E-2</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="9"/>
+      <c r="B29" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>-0.47916666666666669</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="J29" s="1"/>
     </row>
@@ -2829,14 +3026,19 @@
       <c r="J80" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:I2"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="I17" r:id="rId1" display="https://astah.net/support/astah-pro/user-guide/class-diagrams/" xr:uid="{7C32A445-90EE-437F-9496-B44EF63F2338}"/>
     <hyperlink ref="I18" r:id="rId2" display="https://cpnv-es-ngy.gitbook.io/uml-backlog/class-diagram/standards/les-relations" xr:uid="{91F5105D-276F-4EB5-A9C4-C4F8D89CE4EA}"/>
+    <hyperlink ref="I22" r:id="rId3" xr:uid="{B7B62818-4500-4AB2-8FE7-8E07C252C504}"/>
+    <hyperlink ref="I26" r:id="rId4" xr:uid="{3C827EEA-6941-45E7-9714-474050B2BAB0}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="landscape" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2845,8 +3047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E5A45F-AFC1-4C75-BD5B-45FB52BA7D0E}">
   <dimension ref="C3:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2886,7 +3088,7 @@
       </c>
       <c r="D4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!D$3, Tableau1[Durée])</f>
-        <v>0.29513888888888878</v>
+        <v>-0.12847222222222249</v>
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
@@ -2894,7 +3096,7 @@
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>0.13888888888888873</v>
+        <v>0.2013888888888889</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -2902,11 +3104,11 @@
       </c>
       <c r="H4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!H$3, Tableau1[Durée])</f>
-        <v>7.9861111111110994E-2</v>
+        <v>9.7222222222222099E-2</v>
       </c>
       <c r="I4" s="4">
         <f>SUM(D4:H4)</f>
-        <v>0.51388888888888851</v>
+        <v>0.17013888888888851</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -2915,7 +3117,7 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.57432432432432456</v>
+        <v>-0.75510204081632981</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
@@ -2923,7 +3125,7 @@
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.27027027027027017</v>
+        <v>1.1836734693877577</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -2931,11 +3133,11 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>0.15540540540540529</v>
+        <v>0.57142857142857195</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajout des maquettes du jeu
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07330A53-5838-491F-A8A7-7EF4151C78A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324A0F50-E557-4DE7-AAFA-C4C4C1873B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -201,7 +201,22 @@
     <t>Écriture des diagrammes de flux dans le dossier de projet</t>
   </si>
   <si>
-    <t>Création des maquettes pour les menus</t>
+    <t>Réalisation de la maquette du menu principale</t>
+  </si>
+  <si>
+    <t>Création de la maquette du menu priciaple</t>
+  </si>
+  <si>
+    <t>Création de la maquette du menu du chronomètre</t>
+  </si>
+  <si>
+    <t>Création de la maquette d'une partie</t>
+  </si>
+  <si>
+    <t>Création de la maquette pour la fin d'une partie</t>
+  </si>
+  <si>
+    <t>Écriture des maquette dans le dossier de projet</t>
   </si>
 </sst>
 </file>
@@ -300,7 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -332,6 +347,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -718,8 +734,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 57122"/>
-                        <a:gd name="adj2" fmla="val -204500"/>
+                        <a:gd name="adj1" fmla="val 69689"/>
+                        <a:gd name="adj2" fmla="val -177729"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -806,8 +822,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 134499"/>
-                        <a:gd name="adj2" fmla="val -23706"/>
+                        <a:gd name="adj1" fmla="val 125081"/>
+                        <a:gd name="adj2" fmla="val 44709"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -826,7 +842,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-7.5000000000000025E-2"/>
-                  <c:y val="1.3888888888888846E-2"/>
+                  <c:y val="-4.6296296296296511E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -894,8 +910,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 253308"/>
-                        <a:gd name="adj2" fmla="val 74413"/>
+                        <a:gd name="adj1" fmla="val 244367"/>
+                        <a:gd name="adj2" fmla="val 151751"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -913,8 +929,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.0555555555555555E-2"/>
-                  <c:y val="0"/>
+                  <c:x val="2.2222222222222223E-2"/>
+                  <c:y val="-4.6296296296296511E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -982,8 +998,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 147746"/>
-                        <a:gd name="adj2" fmla="val 118033"/>
+                        <a:gd name="adj1" fmla="val 76174"/>
+                        <a:gd name="adj2" fmla="val 189422"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -1083,19 +1099,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-0.75510204081632981</c:v>
+                  <c:v>0.62295081967213106</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1836734693877577</c:v>
+                  <c:v>0.26229508196721329</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57142857142857195</c:v>
+                  <c:v>0.11475409836065564</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2109,8 +2125,8 @@
   </sheetPr>
   <dimension ref="B1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,66 +2770,128 @@
       <c r="C29" s="9">
         <v>0.47916666666666669</v>
       </c>
-      <c r="D29" s="9"/>
+      <c r="D29" s="9">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E29" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>-0.47916666666666669</v>
+        <v>3.1249999999999944E-2</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
+      <c r="B30" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0.52777777777777779</v>
+      </c>
       <c r="E30" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
+      <c r="B31" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="E31" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>5.555555555555558E-2</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
+      <c r="B32" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="E32" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>4.513888888888884E-2</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
+      <c r="B33" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E33" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.7777777777777679E-2</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
+      <c r="B34" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0.6875</v>
+      </c>
       <c r="E34" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="J34" s="1"/>
     </row>
@@ -3036,7 +3114,7 @@
     <hyperlink ref="I26" r:id="rId4" xr:uid="{3C827EEA-6941-45E7-9714-474050B2BAB0}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="landscape" r:id="rId5"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId5"/>
   <tableParts count="1">
     <tablePart r:id="rId6"/>
   </tableParts>
@@ -3045,10 +3123,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E5A45F-AFC1-4C75-BD5B-45FB52BA7D0E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="C3:I80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3088,7 +3169,7 @@
       </c>
       <c r="D4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!D$3, Tableau1[Durée])</f>
-        <v>-0.12847222222222249</v>
+        <v>0.52777777777777746</v>
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
@@ -3096,7 +3177,7 @@
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>0.2013888888888889</v>
+        <v>0.22222222222222227</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -3108,7 +3189,7 @@
       </c>
       <c r="I4" s="4">
         <f>SUM(D4:H4)</f>
-        <v>0.17013888888888851</v>
+        <v>0.84722222222222188</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -3117,7 +3198,7 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>-0.75510204081632981</v>
+        <v>0.62295081967213106</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
@@ -3125,7 +3206,7 @@
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>1.1836734693877577</v>
+        <v>0.26229508196721329</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -3133,11 +3214,11 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>0.57142857142857195</v>
+        <v>0.11475409836065564</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
@@ -3159,6 +3240,7 @@
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
@@ -3393,7 +3475,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="98" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
Ajout des diagrammes de séquences
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324A0F50-E557-4DE7-AAFA-C4C4C1873B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F0A3BF-7AD8-4ECB-9E84-59F118EB9A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -217,6 +217,24 @@
   </si>
   <si>
     <t>Écriture des maquette dans le dossier de projet</t>
+  </si>
+  <si>
+    <t>https://astah.net/support/astah-pro/user-guide/sequence-diagram/</t>
+  </si>
+  <si>
+    <t>Création du diagramme de séquence du déplacement d'une pièce</t>
+  </si>
+  <si>
+    <t>Création du diagramme de séquence du début de la partie</t>
+  </si>
+  <si>
+    <t>Création du diagramme de séquence du fin de jeu</t>
+  </si>
+  <si>
+    <t>Réalisation du diagramme de séquence du fin de jeu</t>
+  </si>
+  <si>
+    <t>Écriture des diagrammes de séquences dans le dossier de projet</t>
   </si>
 </sst>
 </file>
@@ -338,6 +356,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -347,7 +366,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -735,7 +753,7 @@
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
                         <a:gd name="adj1" fmla="val 69689"/>
-                        <a:gd name="adj2" fmla="val -177729"/>
+                        <a:gd name="adj2" fmla="val -210449"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -1099,19 +1117,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.62295081967213106</c:v>
+                  <c:v>1.2173913043478264</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.26229508196721329</c:v>
+                  <c:v>-0.42028985507246397</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11475409836065564</c:v>
+                  <c:v>0.20289855072463758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1779,8 +1797,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}" name="Tableau1" displayName="Tableau1" ref="B3:I35" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="B3:I35" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}" name="Tableau1" displayName="Tableau1" ref="B3:I51" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="B3:I51" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{799BD6A8-A92C-43CC-B95D-FF1653CA16C4}" name="Date" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{1380C259-FA2D-4EA6-91E9-BF1969E7CC18}" name="Début" dataDxfId="6"/>
@@ -2125,8 +2143,8 @@
   </sheetPr>
   <dimension ref="B1:J80"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2144,16 +2162,16 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
@@ -2561,14 +2579,14 @@
         <v>45414</v>
       </c>
       <c r="C20" s="9">
-        <v>0.61458333333333337</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D20" s="9">
         <v>0.62847222222222221</v>
       </c>
       <c r="E20" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>1.388888888888884E-2</v>
+        <v>2.430555555555558E-2</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>3</v>
@@ -2790,14 +2808,14 @@
         <v>45415</v>
       </c>
       <c r="C30" s="9">
-        <v>0.51041666666666663</v>
+        <v>0.5625</v>
       </c>
       <c r="D30" s="9">
-        <v>0.52777777777777779</v>
+        <v>0.57638888888888895</v>
       </c>
       <c r="E30" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>1.736111111111116E-2</v>
+        <v>1.3888888888888951E-2</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>3</v>
@@ -2812,14 +2830,14 @@
         <v>45415</v>
       </c>
       <c r="C31" s="9">
-        <v>0.52777777777777779</v>
+        <v>0.57638888888888895</v>
       </c>
       <c r="D31" s="9">
-        <v>0.58333333333333337</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="E31" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>5.555555555555558E-2</v>
+        <v>2.0833333333333259E-2</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>3</v>
@@ -2834,14 +2852,14 @@
         <v>45415</v>
       </c>
       <c r="C32" s="9">
-        <v>0.58333333333333337</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="D32" s="9">
         <v>0.62847222222222221</v>
       </c>
       <c r="E32" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>4.513888888888884E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>3</v>
@@ -2896,95 +2914,213 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
+      <c r="B35" s="8">
+        <v>45415</v>
+      </c>
+      <c r="C35" s="9">
+        <v>0.6875</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="E35" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
+    <row r="36" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="E36" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="8"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
+      <c r="B37" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C37" s="9">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="E37" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>3.4722222222222154E-2</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="8"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
+      <c r="B38" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D38" s="9">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E38" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="8"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
+      <c r="B39" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="E39" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="8"/>
-      <c r="C40" s="9"/>
+      <c r="B40" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C40" s="9">
+        <v>0.4236111111111111</v>
+      </c>
       <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
+      <c r="E40" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>-0.4236111111111111</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
+      <c r="E41" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E42" s="9"/>
+      <c r="E42" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E43" s="9"/>
+      <c r="E43" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E44" s="9"/>
+      <c r="E44" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E45" s="9"/>
+      <c r="E45" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E46" s="9"/>
+      <c r="E46" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E47" s="9"/>
+      <c r="E47" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E48" s="9"/>
+      <c r="E48" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E49" s="9"/>
+      <c r="E49" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E50" s="9"/>
+      <c r="E50" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E51" s="9"/>
+      <c r="E51" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="5:10" x14ac:dyDescent="0.25">
@@ -3112,11 +3248,12 @@
     <hyperlink ref="I18" r:id="rId2" display="https://cpnv-es-ngy.gitbook.io/uml-backlog/class-diagram/standards/les-relations" xr:uid="{91F5105D-276F-4EB5-A9C4-C4F8D89CE4EA}"/>
     <hyperlink ref="I22" r:id="rId3" xr:uid="{B7B62818-4500-4AB2-8FE7-8E07C252C504}"/>
     <hyperlink ref="I26" r:id="rId4" xr:uid="{3C827EEA-6941-45E7-9714-474050B2BAB0}"/>
+    <hyperlink ref="I36" r:id="rId5" xr:uid="{66F81D81-4ACE-414D-AFA8-FFECF3A4D6D2}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId5"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3128,8 +3265,8 @@
   </sheetPr>
   <dimension ref="C3:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3169,7 +3306,7 @@
       </c>
       <c r="D4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!D$3, Tableau1[Durée])</f>
-        <v>0.52777777777777746</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
@@ -3177,7 +3314,7 @@
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>0.22222222222222227</v>
+        <v>-0.20138888888888884</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -3189,7 +3326,7 @@
       </c>
       <c r="I4" s="4">
         <f>SUM(D4:H4)</f>
-        <v>0.84722222222222188</v>
+        <v>0.4791666666666663</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -3198,7 +3335,7 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.62295081967213106</v>
+        <v>1.2173913043478264</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
@@ -3206,7 +3343,7 @@
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.26229508196721329</v>
+        <v>-0.42028985507246397</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -3214,7 +3351,7 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>0.11475409836065564</v>
+        <v>0.20289855072463758</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>
@@ -3240,7 +3377,7 @@
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="I11" s="13"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
@@ -3475,7 +3612,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="98" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
Ajout de la planification détaillée
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F0A3BF-7AD8-4ECB-9E84-59F118EB9A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB4D5C8-54D8-4A26-AC1B-3D9F89334206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
   <si>
     <t>Date</t>
   </si>
@@ -235,6 +235,27 @@
   </si>
   <si>
     <t>Écriture des diagrammes de séquences dans le dossier de projet</t>
+  </si>
+  <si>
+    <t>Écriture des stratégies de tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Écriture des risques techniques </t>
+  </si>
+  <si>
+    <t>Création de la planification détaillée</t>
+  </si>
+  <si>
+    <t>Réalisation de la planification détaillée</t>
+  </si>
+  <si>
+    <t>Création du projet Unity</t>
+  </si>
+  <si>
+    <t>Configuration des paramètres de Unity</t>
+  </si>
+  <si>
+    <t>Ajout des assets des échecs sur Unity</t>
   </si>
 </sst>
 </file>
@@ -683,8 +704,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.888888888888889E-2"/>
-                  <c:y val="2.3148148148148147E-2"/>
+                  <c:x val="1.1111111111111086E-2"/>
+                  <c:y val="1.3888888888888888E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -752,8 +773,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 69689"/>
-                        <a:gd name="adj2" fmla="val -210449"/>
+                        <a:gd name="adj1" fmla="val 84541"/>
+                        <a:gd name="adj2" fmla="val -127161"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -859,8 +880,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.5000000000000025E-2"/>
-                  <c:y val="-4.6296296296296511E-3"/>
+                  <c:x val="-0.05"/>
+                  <c:y val="-1.8518518518518517E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -928,8 +949,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 244367"/>
-                        <a:gd name="adj2" fmla="val 151751"/>
+                        <a:gd name="adj1" fmla="val 178795"/>
+                        <a:gd name="adj2" fmla="val 166624"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -947,8 +968,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="2.2222222222222223E-2"/>
-                  <c:y val="-4.6296296296296511E-3"/>
+                  <c:x val="4.7222222222222172E-2"/>
+                  <c:y val="9.2592592592592587E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -1016,8 +1037,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 76174"/>
-                        <a:gd name="adj2" fmla="val 189422"/>
+                        <a:gd name="adj1" fmla="val 4602"/>
+                        <a:gd name="adj2" fmla="val 168600"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -1117,19 +1138,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.2173913043478264</c:v>
+                  <c:v>0.56582633053221287</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>9.5238095238095163E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.42028985507246397</c:v>
+                  <c:v>0.26050420168067234</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20289855072463758</c:v>
+                  <c:v>7.8431372549019537E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2143,8 +2164,8 @@
   </sheetPr>
   <dimension ref="B1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2913,7 +2934,7 @@
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="8">
         <v>45415</v>
       </c>
@@ -2930,9 +2951,15 @@
       <c r="F35" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="8">
         <v>45418</v>
       </c>
@@ -2950,10 +2977,7 @@
         <v>3</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J36" s="1"/>
     </row>
@@ -2975,7 +2999,7 @@
         <v>3</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J37" s="1"/>
     </row>
@@ -2997,7 +3021,7 @@
         <v>3</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J38" s="1"/>
     </row>
@@ -3009,17 +3033,17 @@
         <v>0.40972222222222227</v>
       </c>
       <c r="D39" s="9">
-        <v>0.4236111111111111</v>
+        <v>0.43055555555555558</v>
       </c>
       <c r="E39" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>1.388888888888884E-2</v>
+        <v>2.0833333333333315E-2</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J39" s="1"/>
     </row>
@@ -3028,99 +3052,176 @@
         <v>45418</v>
       </c>
       <c r="C40" s="9">
-        <v>0.4236111111111111</v>
-      </c>
-      <c r="D40" s="9"/>
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D40" s="9">
+        <v>0.46527777777777773</v>
+      </c>
       <c r="E40" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>-0.4236111111111111</v>
+        <v>3.4722222222222154E-2</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="8"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
+      <c r="B41" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C41" s="9">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="D41" s="9">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E41" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="D42" s="9">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="E42" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C43" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D43" s="9">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="E43" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>6.5972222222222265E-2</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0.4826388888888889</v>
+      </c>
       <c r="E44" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C45" s="9">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D45" s="9">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E45" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C46" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="D46" s="9">
+        <v>0.57986111111111105</v>
+      </c>
       <c r="E46" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E47" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E48" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="E48" s="9"/>
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E49" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="E49" s="9"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E50" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="E50" s="9"/>
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E51" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="E51" s="9"/>
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="5:10" x14ac:dyDescent="0.25">
@@ -3248,7 +3349,7 @@
     <hyperlink ref="I18" r:id="rId2" display="https://cpnv-es-ngy.gitbook.io/uml-backlog/class-diagram/standards/les-relations" xr:uid="{91F5105D-276F-4EB5-A9C4-C4F8D89CE4EA}"/>
     <hyperlink ref="I22" r:id="rId3" xr:uid="{B7B62818-4500-4AB2-8FE7-8E07C252C504}"/>
     <hyperlink ref="I26" r:id="rId4" xr:uid="{3C827EEA-6941-45E7-9714-474050B2BAB0}"/>
-    <hyperlink ref="I36" r:id="rId5" xr:uid="{66F81D81-4ACE-414D-AFA8-FFECF3A4D6D2}"/>
+    <hyperlink ref="I35" r:id="rId5" xr:uid="{66F81D81-4ACE-414D-AFA8-FFECF3A4D6D2}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId6"/>
@@ -3266,7 +3367,7 @@
   <dimension ref="C3:I80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3306,15 +3407,15 @@
       </c>
       <c r="D4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!D$3, Tableau1[Durée])</f>
-        <v>0.58333333333333304</v>
+        <v>0.70138888888888862</v>
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>0</v>
+        <v>0.11805555555555541</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>-0.20138888888888884</v>
+        <v>0.32291666666666663</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -3326,7 +3427,7 @@
       </c>
       <c r="I4" s="4">
         <f>SUM(D4:H4)</f>
-        <v>0.4791666666666663</v>
+        <v>1.2395833333333328</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -3335,15 +3436,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>1.2173913043478264</v>
+        <v>0.56582633053221287</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0</v>
+        <v>9.5238095238095163E-2</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>-0.42028985507246397</v>
+        <v>0.26050420168067234</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -3351,11 +3452,11 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>0.20289855072463758</v>
+        <v>7.8431372549019537E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Création du projet Unity
Implémentation du menu et de l'échiquier
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB4D5C8-54D8-4A26-AC1B-3D9F89334206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7EC217-4F77-453F-9EC6-AF609D6DAA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -256,6 +256,24 @@
   </si>
   <si>
     <t>Ajout des assets des échecs sur Unity</t>
+  </si>
+  <si>
+    <t>Création des scénarios de tests</t>
+  </si>
+  <si>
+    <t>Réalisation des scénarios de tests</t>
+  </si>
+  <si>
+    <t>Ajout d'un menu temporaire du jeu</t>
+  </si>
+  <si>
+    <t>Ajout des scènes dans Unity</t>
+  </si>
+  <si>
+    <t>Création de la classe de l'échiquier et mise en place de la scène</t>
+  </si>
+  <si>
+    <t>Implémentation de l'initialisation de l'échiquier</t>
   </si>
 </sst>
 </file>
@@ -1138,19 +1156,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.56582633053221287</c:v>
+                  <c:v>0.53196347031963476</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.5238095238095163E-2</c:v>
+                  <c:v>0.18264840182648398</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.26050420168067234</c:v>
+                  <c:v>0.22146118721461189</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.8431372549019537E-2</c:v>
+                  <c:v>6.3926940639269347E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1818,8 +1836,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}" name="Tableau1" displayName="Tableau1" ref="B3:I51" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="B3:I51" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}" name="Tableau1" displayName="Tableau1" ref="B3:I63" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="B3:I63" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{799BD6A8-A92C-43CC-B95D-FF1653CA16C4}" name="Date" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{1380C259-FA2D-4EA6-91E9-BF1969E7CC18}" name="Début" dataDxfId="6"/>
@@ -2164,8 +2182,8 @@
   </sheetPr>
   <dimension ref="B1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3202,77 +3220,230 @@
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="8"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
+      <c r="B47" s="8">
+        <v>45418</v>
+      </c>
+      <c r="C47" s="9">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="D47" s="9">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E47" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>4.861111111111116E-2</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E48" s="9"/>
+      <c r="B48" s="8">
+        <v>45419</v>
+      </c>
+      <c r="C48" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D48" s="9">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="E48" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>5.902777777777779E-2</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E49" s="9"/>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="8">
+        <v>45419</v>
+      </c>
+      <c r="C49" s="9">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D49" s="9">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E49" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E50" s="9"/>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="8">
+        <v>45419</v>
+      </c>
+      <c r="C50" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D50" s="9">
+        <v>0.46875</v>
+      </c>
+      <c r="E50" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>5.9027777777777735E-2</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E51" s="9"/>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="8">
+        <v>45419</v>
+      </c>
+      <c r="C51" s="9">
+        <v>0.46875</v>
+      </c>
+      <c r="D51" s="9">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E51" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E52" s="9"/>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="8">
+        <v>45419</v>
+      </c>
+      <c r="C52" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="D52" s="9">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="E52" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E53" s="9"/>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="8">
+        <v>45419</v>
+      </c>
+      <c r="C53" s="9">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D53" s="9">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E53" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E54" s="9"/>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E54" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J54" s="1"/>
     </row>
-    <row r="55" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E55" s="9"/>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E55" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E56" s="9"/>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="8">
+        <v>45425</v>
+      </c>
+      <c r="E56" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E57" s="9"/>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E57" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E58" s="9"/>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E58" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E59" s="9"/>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E59" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J59" s="1"/>
     </row>
-    <row r="60" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E60" s="9"/>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E60" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E61" s="9"/>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E61" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J61" s="1"/>
     </row>
-    <row r="62" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E62" s="9"/>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E62" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E63" s="9"/>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E63" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E64" s="9"/>
       <c r="J64" s="1"/>
     </row>
@@ -3407,15 +3578,15 @@
       </c>
       <c r="D4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!D$3, Tableau1[Durée])</f>
-        <v>0.70138888888888862</v>
+        <v>0.80902777777777757</v>
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>0.11805555555555541</v>
+        <v>0.27777777777777762</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>0.32291666666666663</v>
+        <v>0.33680555555555547</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -3427,7 +3598,7 @@
       </c>
       <c r="I4" s="4">
         <f>SUM(D4:H4)</f>
-        <v>1.2395833333333328</v>
+        <v>1.5208333333333328</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -3436,15 +3607,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.56582633053221287</v>
+        <v>0.53196347031963476</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>9.5238095238095163E-2</v>
+        <v>0.18264840182648398</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.26050420168067234</v>
+        <v>0.22146118721461189</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -3452,11 +3623,11 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>7.8431372549019537E-2</v>
+        <v>6.3926940639269347E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajout des scripts pour les pièces
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7EC217-4F77-453F-9EC6-AF609D6DAA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3E692C-E35B-49DE-95CE-39FBCC818671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
+    <workbookView xWindow="8700" yWindow="2085" windowWidth="16035" windowHeight="13290" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>Implémentation de l'initialisation de l'échiquier</t>
+  </si>
+  <si>
+    <t>https://docs.unity3d.com/Manual/InstantiatingPrefabs.html</t>
+  </si>
+  <si>
+    <t>Rédaction de la planification</t>
+  </si>
+  <si>
+    <t>Création des scripts pour les pièces</t>
   </si>
 </sst>
 </file>
@@ -1156,19 +1165,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.53196347031963476</c:v>
+                  <c:v>0.52125279642058175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18264840182648398</c:v>
+                  <c:v>0.18344519015659955</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22146118721461189</c:v>
+                  <c:v>0.23266219239373606</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.3926940639269347E-2</c:v>
+                  <c:v>6.2639821029082721E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2182,8 +2191,8 @@
   </sheetPr>
   <dimension ref="B1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3349,6 +3358,9 @@
       <c r="G52" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="I52" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
@@ -3371,23 +3383,32 @@
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="8">
+        <v>45419</v>
+      </c>
+      <c r="C54" s="9">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D54" s="9">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="E54" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" s="8">
+        <v>45425</v>
+      </c>
+      <c r="E55" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
-      <c r="J54" s="1"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E55" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="8">
-        <v>45425</v>
-      </c>
       <c r="E56" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
@@ -3402,16 +3423,46 @@
       <c r="J57" s="1"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="8">
+        <v>45428</v>
+      </c>
+      <c r="C58" s="9">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D58" s="9">
+        <v>0.3923611111111111</v>
+      </c>
       <c r="E58" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="8">
+        <v>45428</v>
+      </c>
+      <c r="C59" s="9">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D59" s="9">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="E59" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="J59" s="1"/>
     </row>
@@ -3521,11 +3572,12 @@
     <hyperlink ref="I22" r:id="rId3" xr:uid="{B7B62818-4500-4AB2-8FE7-8E07C252C504}"/>
     <hyperlink ref="I26" r:id="rId4" xr:uid="{3C827EEA-6941-45E7-9714-474050B2BAB0}"/>
     <hyperlink ref="I35" r:id="rId5" xr:uid="{66F81D81-4ACE-414D-AFA8-FFECF3A4D6D2}"/>
+    <hyperlink ref="I52" r:id="rId6" xr:uid="{AA195AD4-FC1E-47FD-97C8-F3CA670D3842}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId6"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3582,11 +3634,11 @@
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>0.27777777777777762</v>
+        <v>0.2847222222222221</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>0.33680555555555547</v>
+        <v>0.36111111111111099</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -3598,7 +3650,7 @@
       </c>
       <c r="I4" s="4">
         <f>SUM(D4:H4)</f>
-        <v>1.5208333333333328</v>
+        <v>1.5520833333333326</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -3607,15 +3659,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.53196347031963476</v>
+        <v>0.52125279642058175</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.18264840182648398</v>
+        <v>0.18344519015659955</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.22146118721461189</v>
+        <v>0.23266219239373606</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -3623,7 +3675,7 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>6.3926940639269347E-2</v>
+        <v>6.2639821029082721E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>

</xml_diff>

<commit_message>
Mise à jour du journal de travail et ajout des textures des pièces
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3E692C-E35B-49DE-95CE-39FBCC818671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9A9B6D-3254-4D12-B44D-72402F8A5FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="2085" windowWidth="16035" windowHeight="13290" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>Création des scripts pour les pièces</t>
+  </si>
+  <si>
+    <t>Ajout des sprites pour les pièces</t>
   </si>
 </sst>
 </file>
@@ -1165,19 +1168,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.52125279642058175</c:v>
+                  <c:v>0.46737213403880062</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18344519015659955</c:v>
+                  <c:v>0.27336860670194013</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.23266219239373606</c:v>
+                  <c:v>0.20987654320987661</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.2639821029082721E-2</c:v>
+                  <c:v>4.9382716049382672E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1845,8 +1848,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}" name="Tableau1" displayName="Tableau1" ref="B3:I63" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="B3:I63" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}" name="Tableau1" displayName="Tableau1" ref="B3:I106" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="B3:I106" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{799BD6A8-A92C-43CC-B95D-FF1653CA16C4}" name="Date" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{1380C259-FA2D-4EA6-91E9-BF1969E7CC18}" name="Début" dataDxfId="6"/>
@@ -2189,10 +2192,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J80"/>
+  <dimension ref="B1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2994,11 +2997,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D36" s="9">
-        <v>0.34722222222222227</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="E36" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>1.3888888888888951E-2</v>
+        <v>6.5972222222222265E-2</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>3</v>
@@ -3013,14 +3016,14 @@
         <v>45418</v>
       </c>
       <c r="C37" s="9">
-        <v>0.34722222222222227</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="D37" s="9">
-        <v>0.38194444444444442</v>
+        <v>0.46180555555555558</v>
       </c>
       <c r="E37" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>3.4722222222222154E-2</v>
+        <v>5.2083333333333315E-2</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>3</v>
@@ -3035,14 +3038,14 @@
         <v>45418</v>
       </c>
       <c r="C38" s="9">
-        <v>0.38194444444444442</v>
+        <v>0.46180555555555558</v>
       </c>
       <c r="D38" s="9">
-        <v>0.39930555555555558</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="E38" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>1.736111111111116E-2</v>
+        <v>4.8611111111111049E-2</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>3</v>
@@ -3057,14 +3060,14 @@
         <v>45418</v>
       </c>
       <c r="C39" s="9">
-        <v>0.40972222222222227</v>
+        <v>0.5625</v>
       </c>
       <c r="D39" s="9">
-        <v>0.43055555555555558</v>
+        <v>0.62847222222222221</v>
       </c>
       <c r="E39" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>2.0833333333333315E-2</v>
+        <v>6.597222222222221E-2</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>2</v>
@@ -3076,51 +3079,51 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="8">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="C40" s="9">
-        <v>0.43055555555555558</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D40" s="9">
-        <v>0.46527777777777773</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="E40" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>3.4722222222222154E-2</v>
+        <v>6.5972222222222265E-2</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="8">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="C41" s="9">
-        <v>0.46527777777777773</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="D41" s="9">
         <v>0.51041666666666663</v>
       </c>
       <c r="E41" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>4.5138888888888895E-2</v>
+        <v>0.10069444444444436</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="8">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="C42" s="9">
         <v>0.5625</v>
@@ -3136,431 +3139,567 @@
         <v>3</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="8">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="C43" s="9">
-        <v>0.33333333333333331</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="D43" s="9">
-        <v>0.39930555555555558</v>
+        <v>0.70486111111111116</v>
       </c>
       <c r="E43" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>6.5972222222222265E-2</v>
+        <v>6.597222222222221E-2</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="8">
-        <v>45418</v>
+        <v>45425</v>
       </c>
       <c r="C44" s="9">
-        <v>0.40972222222222227</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D44" s="9">
-        <v>0.4826388888888889</v>
+        <v>0.34375</v>
       </c>
       <c r="E44" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>7.291666666666663E-2</v>
+        <v>1.0416666666666685E-2</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="8">
-        <v>45418</v>
+        <v>45425</v>
       </c>
       <c r="C45" s="9">
-        <v>0.4826388888888889</v>
+        <v>0.34375</v>
       </c>
       <c r="D45" s="9">
-        <v>0.51041666666666663</v>
+        <v>0.36805555555555558</v>
       </c>
       <c r="E45" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>2.7777777777777735E-2</v>
+        <v>2.430555555555558E-2</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="8">
-        <v>45418</v>
+        <v>45425</v>
       </c>
       <c r="C46" s="9">
-        <v>0.5625</v>
+        <v>0.36805555555555558</v>
       </c>
       <c r="D46" s="9">
-        <v>0.57986111111111105</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="E46" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>1.7361111111111049E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="8">
-        <v>45418</v>
+        <v>45425</v>
       </c>
       <c r="C47" s="9">
-        <v>0.57986111111111105</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="D47" s="9">
-        <v>0.62847222222222221</v>
+        <v>0.46180555555555558</v>
       </c>
       <c r="E47" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>4.861111111111116E-2</v>
+        <v>5.2083333333333315E-2</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="8">
-        <v>45419</v>
+        <v>45425</v>
       </c>
       <c r="C48" s="9">
-        <v>0.33333333333333331</v>
+        <v>0.46180555555555558</v>
       </c>
       <c r="D48" s="9">
-        <v>0.3923611111111111</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="E48" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>5.902777777777779E-2</v>
+        <v>1.7361111111111105E-2</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="8">
-        <v>45419</v>
+        <v>45425</v>
       </c>
       <c r="C49" s="9">
-        <v>0.3923611111111111</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="D49" s="9">
-        <v>0.39930555555555558</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="E49" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>6.9444444444444753E-3</v>
+        <v>3.1249999999999944E-2</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="8">
-        <v>45419</v>
+        <v>45425</v>
       </c>
       <c r="C50" s="9">
-        <v>0.40972222222222227</v>
+        <v>0.5625</v>
       </c>
       <c r="D50" s="9">
-        <v>0.46875</v>
+        <v>0.62847222222222221</v>
       </c>
       <c r="E50" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>5.9027777777777735E-2</v>
+        <v>6.597222222222221E-2</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="8">
-        <v>45419</v>
+        <v>45426</v>
       </c>
       <c r="C51" s="9">
-        <v>0.46875</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D51" s="9">
-        <v>0.51041666666666663</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="E51" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>4.166666666666663E-2</v>
+        <v>0.28125000000000006</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="8">
-        <v>45419</v>
+        <v>45418</v>
       </c>
       <c r="C52" s="9">
-        <v>0.5625</v>
+        <v>0.43055555555555558</v>
       </c>
       <c r="D52" s="9">
-        <v>0.61458333333333337</v>
+        <v>0.46527777777777773</v>
       </c>
       <c r="E52" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>5.208333333333337E-2</v>
+        <v>3.4722222222222154E-2</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="8">
-        <v>45419</v>
+        <v>45428</v>
       </c>
       <c r="C53" s="9">
-        <v>0.61458333333333337</v>
+        <v>0.36805555555555558</v>
       </c>
       <c r="D53" s="9">
-        <v>0.62847222222222221</v>
+        <v>0.3923611111111111</v>
       </c>
       <c r="E53" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>1.388888888888884E-2</v>
+        <v>2.4305555555555525E-2</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="G53" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="8">
-        <v>45419</v>
+        <v>45428</v>
       </c>
       <c r="C54" s="9">
-        <v>0.63888888888888895</v>
+        <v>0.3923611111111111</v>
       </c>
       <c r="D54" s="9">
-        <v>0.70486111111111116</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="E54" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>6.597222222222221E-2</v>
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="8">
-        <v>45425</v>
+        <v>45428</v>
+      </c>
+      <c r="C55" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D55" s="9">
+        <v>0.44444444444444442</v>
       </c>
       <c r="E55" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>3.4722222222222154E-2</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E56" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="E56" s="9"/>
       <c r="J56" s="1"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E57" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="E57" s="9"/>
       <c r="J57" s="1"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="8">
-        <v>45428</v>
-      </c>
-      <c r="C58" s="9">
-        <v>0.36805555555555558</v>
-      </c>
-      <c r="D58" s="9">
-        <v>0.3923611111111111</v>
-      </c>
-      <c r="E58" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>2.4305555555555525E-2</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="E58" s="9"/>
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="8">
-        <v>45428</v>
-      </c>
-      <c r="C59" s="9">
-        <v>0.3923611111111111</v>
-      </c>
-      <c r="D59" s="9">
-        <v>0.39930555555555558</v>
-      </c>
-      <c r="E59" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>6.9444444444444753E-3</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E59" s="9"/>
       <c r="J59" s="1"/>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E60" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="E60" s="9"/>
       <c r="J60" s="1"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E61" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="E61" s="9"/>
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E62" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="E62" s="9"/>
       <c r="J62" s="1"/>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E63" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="E63" s="9"/>
       <c r="J63" s="1"/>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E64" s="9"/>
       <c r="J64" s="1"/>
     </row>
-    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E65" s="9"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E66" s="9"/>
       <c r="J66" s="1"/>
     </row>
-    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E67" s="9"/>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E68" s="9"/>
       <c r="J68" s="1"/>
     </row>
-    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E69" s="9"/>
       <c r="J69" s="1"/>
     </row>
-    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E70" s="9"/>
       <c r="J70" s="1"/>
     </row>
-    <row r="71" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B71" s="8"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
       <c r="E71" s="9"/>
       <c r="J71" s="1"/>
     </row>
-    <row r="72" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B72" s="8"/>
       <c r="E72" s="9"/>
       <c r="J72" s="1"/>
     </row>
-    <row r="73" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E73" s="9"/>
       <c r="J73" s="1"/>
     </row>
-    <row r="74" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E74" s="9"/>
       <c r="J74" s="1"/>
     </row>
-    <row r="75" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E75" s="9"/>
       <c r="J75" s="1"/>
     </row>
-    <row r="76" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E76" s="9"/>
       <c r="J76" s="1"/>
     </row>
-    <row r="77" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E77" s="9"/>
       <c r="J77" s="1"/>
     </row>
-    <row r="78" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E78" s="9"/>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E78" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J78" s="1"/>
     </row>
-    <row r="79" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E79" s="9"/>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E79" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J79" s="1"/>
     </row>
-    <row r="80" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E80" s="9"/>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E80" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
       <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E81" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E83" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E85" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E87" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E89" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E90" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E99" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E100" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E101" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E102" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E103" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E104" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E105" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E106" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3572,7 +3711,7 @@
     <hyperlink ref="I22" r:id="rId3" xr:uid="{B7B62818-4500-4AB2-8FE7-8E07C252C504}"/>
     <hyperlink ref="I26" r:id="rId4" xr:uid="{3C827EEA-6941-45E7-9714-474050B2BAB0}"/>
     <hyperlink ref="I35" r:id="rId5" xr:uid="{66F81D81-4ACE-414D-AFA8-FFECF3A4D6D2}"/>
-    <hyperlink ref="I52" r:id="rId6" xr:uid="{AA195AD4-FC1E-47FD-97C8-F3CA670D3842}"/>
+    <hyperlink ref="I51" r:id="rId6" xr:uid="{AA195AD4-FC1E-47FD-97C8-F3CA670D3842}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId7"/>
@@ -3630,15 +3769,15 @@
       </c>
       <c r="D4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!D$3, Tableau1[Durée])</f>
-        <v>0.80902777777777757</v>
+        <v>0.9201388888888884</v>
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>0.2847222222222221</v>
+        <v>0.53819444444444442</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>0.36111111111111099</v>
+        <v>0.41319444444444442</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -3650,7 +3789,7 @@
       </c>
       <c r="I4" s="4">
         <f>SUM(D4:H4)</f>
-        <v>1.5520833333333326</v>
+        <v>1.9687499999999993</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -3659,15 +3798,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.52125279642058175</v>
+        <v>0.46737213403880062</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.18344519015659955</v>
+        <v>0.27336860670194013</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.23266219239373606</v>
+        <v>0.20987654320987661</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -3675,7 +3814,7 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>6.2639821029082721E-2</v>
+        <v>4.9382716049382672E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>

</xml_diff>

<commit_message>
Implémentation du système de mouvement généré et de saisie de la souris
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAD6C20-E61F-4D2D-8D65-C393C32B55FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061B3CEF-DFE6-4661-997F-3B3BE551C2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>https://docs.unity3d.com/Manual/sprite-automatic-slicing.html</t>
+  </si>
+  <si>
+    <t>Rédaction de l'implémentation des pièces</t>
+  </si>
+  <si>
+    <t>Implémentation du mouvement des pièces</t>
   </si>
 </sst>
 </file>
@@ -1189,19 +1195,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.41021671826625383</c:v>
+                  <c:v>0.64950980392156865</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.30650154798761625</c:v>
+                  <c:v>0.19117647058823539</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21981424148606823</c:v>
+                  <c:v>5.8823529411764726E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.3467492260061875E-2</c:v>
+                  <c:v>0.10049019607843131</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2215,8 +2221,8 @@
   </sheetPr>
   <dimension ref="B1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3596,16 +3602,40 @@
       <c r="J62" s="1"/>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="8">
+        <v>45429</v>
+      </c>
+      <c r="C63" s="9">
+        <v>0.40972222222222227</v>
+      </c>
       <c r="E63" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>-0.40972222222222227</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="J63" s="1"/>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="8">
+        <v>45429</v>
+      </c>
+      <c r="C64" s="9">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="E64" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>-0.41666666666666669</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="J64" s="1"/>
     </row>
@@ -3955,11 +3985,11 @@
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>0.6875</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>0.49305555555555558</v>
+        <v>8.3333333333333315E-2</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -3971,7 +4001,7 @@
       </c>
       <c r="I4" s="4">
         <f>SUM(D4:H4)</f>
-        <v>2.2430555555555545</v>
+        <v>1.4166666666666659</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -3980,15 +4010,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.41021671826625383</v>
+        <v>0.64950980392156865</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.30650154798761625</v>
+        <v>0.19117647058823539</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.21981424148606823</v>
+        <v>5.8823529411764726E-2</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -3996,7 +4026,7 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>6.3467492260061875E-2</v>
+        <v>0.10049019607843131</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>

</xml_diff>

<commit_message>
Rectification d'erreur concernant le scale de la camera
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061B3CEF-DFE6-4661-997F-3B3BE551C2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E853D561-59A1-4A0F-B49D-7F96791270F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="93">
   <si>
     <t>Date</t>
   </si>
@@ -309,10 +309,13 @@
     <t>https://docs.unity3d.com/Manual/sprite-automatic-slicing.html</t>
   </si>
   <si>
-    <t>Rédaction de l'implémentation des pièces</t>
-  </si>
-  <si>
-    <t>Implémentation du mouvement des pièces</t>
+    <t>Implémentation de la génération du mouvement des pièces</t>
+  </si>
+  <si>
+    <t>Implémentation de la saisie de la souris</t>
+  </si>
+  <si>
+    <t>Résolution de problème avec la saisie de la souris</t>
   </si>
 </sst>
 </file>
@@ -1195,19 +1198,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.64950980392156865</c:v>
+                  <c:v>0.37166900420757354</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19117647058823539</c:v>
+                  <c:v>0.37166900420757371</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8823529411764726E-2</c:v>
+                  <c:v>0.19915848527349236</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10049019607843131</c:v>
+                  <c:v>5.7503506311360392E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2221,8 +2224,8 @@
   </sheetPr>
   <dimension ref="B1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3608,12 +3611,15 @@
       <c r="C63" s="9">
         <v>0.40972222222222227</v>
       </c>
+      <c r="D63" s="9">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E63" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>-0.40972222222222227</v>
+        <v>0.10069444444444436</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>90</v>
@@ -3625,11 +3631,14 @@
         <v>45429</v>
       </c>
       <c r="C64" s="9">
-        <v>0.41666666666666669</v>
+        <v>0.5625</v>
+      </c>
+      <c r="D64" s="9">
+        <v>0.62847222222222221</v>
       </c>
       <c r="E64" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>-0.41666666666666669</v>
+        <v>6.597222222222221E-2</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>4</v>
@@ -3640,17 +3649,29 @@
       <c r="J64" s="1"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" s="8">
+        <v>45429</v>
+      </c>
+      <c r="C65" s="9">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D65" s="9">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="E65" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="J65" s="1"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E66" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="E66" s="9"/>
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
@@ -3985,11 +4006,11 @@
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>0.27083333333333331</v>
+        <v>0.92013888888888884</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -4001,7 +4022,7 @@
       </c>
       <c r="I4" s="4">
         <f>SUM(D4:H4)</f>
-        <v>1.4166666666666659</v>
+        <v>2.4756944444444438</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -4010,15 +4031,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.64950980392156865</v>
+        <v>0.37166900420757354</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.19117647058823539</v>
+        <v>0.37166900420757371</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>5.8823529411764726E-2</v>
+        <v>0.19915848527349236</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -4026,7 +4047,7 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>0.10049019607843131</v>
+        <v>5.7503506311360392E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>

</xml_diff>

<commit_message>
Déplacement des fonctionalités de la saisie dans un manager séparé
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E853D561-59A1-4A0F-B49D-7F96791270F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A90B61-EEC3-45B8-8BF3-2FBBC52A0271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -316,16 +316,23 @@
   </si>
   <si>
     <t>Résolution de problème avec la saisie de la souris</t>
+  </si>
+  <si>
+    <t>Amélioratoin du dossier de projet</t>
+  </si>
+  <si>
+    <t>Coup de mou pour le 06 et le 07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="169" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +352,12 @@
       <b/>
       <sz val="36"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -414,7 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -447,6 +460,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -833,8 +847,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 84541"/>
-                        <a:gd name="adj2" fmla="val -127161"/>
+                        <a:gd name="adj1" fmla="val 41129"/>
+                        <a:gd name="adj2" fmla="val -150957"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -1198,19 +1212,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.37166900420757354</c:v>
+                  <c:v>0.38297872340425532</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.37166900420757371</c:v>
+                  <c:v>0.31347517730496466</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19915848527349236</c:v>
+                  <c:v>0.24539007092198595</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.7503506311360392E-2</c:v>
+                  <c:v>5.8156028368794292E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2224,8 +2238,8 @@
   </sheetPr>
   <dimension ref="B1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3039,6 +3053,9 @@
       <c r="G36" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="H36" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
@@ -3061,6 +3078,9 @@
       <c r="G37" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="H37" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
@@ -3083,6 +3103,9 @@
       <c r="G38" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="H38" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
@@ -3105,6 +3128,9 @@
       <c r="G39" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="H39" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
@@ -3127,6 +3153,9 @@
       <c r="G40" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="H40" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
@@ -3149,6 +3178,9 @@
       <c r="G41" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="H41" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
@@ -3171,6 +3203,9 @@
       <c r="G42" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="H42" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
@@ -3193,6 +3228,9 @@
       <c r="G43" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="H43" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
@@ -3225,11 +3263,11 @@
         <v>0.34375</v>
       </c>
       <c r="D45" s="9">
-        <v>0.36805555555555558</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="E45" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>2.430555555555558E-2</v>
+        <v>5.555555555555558E-2</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>4</v>
@@ -3244,14 +3282,14 @@
         <v>45425</v>
       </c>
       <c r="C46" s="9">
-        <v>0.36805555555555558</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="D46" s="9">
-        <v>0.39930555555555558</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E46" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>3.125E-2</v>
+        <v>3.4722222222222154E-2</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>3</v>
@@ -3266,14 +3304,14 @@
         <v>45425</v>
       </c>
       <c r="C47" s="9">
-        <v>0.40972222222222227</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D47" s="9">
-        <v>0.46180555555555558</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="E47" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>5.2083333333333315E-2</v>
+        <v>6.597222222222221E-2</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>3</v>
@@ -3288,14 +3326,14 @@
         <v>45425</v>
       </c>
       <c r="C48" s="9">
-        <v>0.46180555555555558</v>
+        <v>0.5625</v>
       </c>
       <c r="D48" s="9">
-        <v>0.47916666666666669</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="E48" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>1.7361111111111105E-2</v>
+        <v>1.041666666666663E-2</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>4</v>
@@ -3310,14 +3348,14 @@
         <v>45425</v>
       </c>
       <c r="C49" s="9">
-        <v>0.47916666666666669</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="D49" s="9">
-        <v>0.51041666666666663</v>
+        <v>0.62847222222222221</v>
       </c>
       <c r="E49" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>3.1249999999999944E-2</v>
+        <v>5.555555555555558E-2</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>4</v>
@@ -3329,17 +3367,17 @@
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="8">
-        <v>45425</v>
+        <v>45426</v>
       </c>
       <c r="C50" s="9">
-        <v>0.5625</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D50" s="9">
-        <v>0.62847222222222221</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="E50" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>6.597222222222221E-2</v>
+        <v>6.5972222222222265E-2</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>4</v>
@@ -3354,14 +3392,14 @@
         <v>45426</v>
       </c>
       <c r="C51" s="9">
-        <v>0.33333333333333331</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="D51" s="9">
-        <v>0.39930555555555558</v>
+        <v>0.47569444444444442</v>
       </c>
       <c r="E51" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>6.5972222222222265E-2</v>
+        <v>6.5972222222222154E-2</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>2</v>
@@ -3379,14 +3417,14 @@
         <v>45426</v>
       </c>
       <c r="C52" s="9">
-        <v>0.40972222222222227</v>
+        <v>0.47569444444444442</v>
       </c>
       <c r="D52" s="9">
-        <v>0.70486111111111116</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="E52" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0.2951388888888889</v>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>4</v>
@@ -3397,28 +3435,46 @@
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E53" s="9"/>
+      <c r="B53" s="8">
+        <v>45426</v>
+      </c>
+      <c r="C53" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="D53" s="9">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E53" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="8">
-        <v>45428</v>
+        <v>45426</v>
       </c>
       <c r="C54" s="9">
-        <v>0.36805555555555558</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="D54" s="9">
-        <v>0.3923611111111111</v>
+        <v>0.70486111111111116</v>
       </c>
       <c r="E54" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>2.4305555555555525E-2</v>
+        <v>6.597222222222221E-2</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J54" s="1"/>
     </row>
@@ -3427,20 +3483,20 @@
         <v>45428</v>
       </c>
       <c r="C55" s="9">
-        <v>0.3923611111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D55" s="9">
         <v>0.39930555555555558</v>
       </c>
       <c r="E55" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>6.9444444444444753E-3</v>
+        <v>6.5972222222222265E-2</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="J55" s="1"/>
     </row>
@@ -3936,6 +3992,7 @@
   <mergeCells count="1">
     <mergeCell ref="B2:I2"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I17" r:id="rId1" display="https://astah.net/support/astah-pro/user-guide/class-diagrams/" xr:uid="{7C32A445-90EE-437F-9496-B44EF63F2338}"/>
     <hyperlink ref="I18" r:id="rId2" display="https://cpnv-es-ngy.gitbook.io/uml-backlog/class-diagram/standards/les-relations" xr:uid="{91F5105D-276F-4EB5-A9C4-C4F8D89CE4EA}"/>
@@ -3962,7 +4019,7 @@
   <dimension ref="C3:I80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4002,15 +4059,15 @@
       </c>
       <c r="D4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!D$3, Tableau1[Durée])</f>
-        <v>0.9201388888888884</v>
+        <v>0.93749999999999944</v>
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>0.92013888888888884</v>
+        <v>0.76736111111111094</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>0.49305555555555558</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -4020,9 +4077,9 @@
         <f>SUMIF(Tableau1[Sujet], Sheet1!H$3, Tableau1[Durée])</f>
         <v>0.14236111111111094</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="14">
         <f>SUM(D4:H4)</f>
-        <v>2.4756944444444438</v>
+        <v>2.4479166666666652</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -4031,15 +4088,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.37166900420757354</v>
+        <v>0.38297872340425532</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.37166900420757371</v>
+        <v>0.31347517730496466</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.19915848527349236</v>
+        <v>0.24539007092198595</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -4047,11 +4104,11 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>5.7503506311360392E-2</v>
+        <v>5.8156028368794292E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajout de la prévision du mouvement des pièces
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A90B61-EEC3-45B8-8BF3-2FBBC52A0271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F51373-BD0C-40FD-BC2F-B7F76E5C78D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -322,6 +322,27 @@
   </si>
   <si>
     <t>Coup de mou pour le 06 et le 07</t>
+  </si>
+  <si>
+    <t>Déplacement de la fonctionalité de la saisie dans un script apart</t>
+  </si>
+  <si>
+    <t>Implémentation du déplacement des pièces</t>
+  </si>
+  <si>
+    <t>https://discussions.unity.com/t/how-delete-or-remove-a-component-of-an-gameobject/60182</t>
+  </si>
+  <si>
+    <t>https://docs.unity3d.com/Packages/com.unity.inputsystem@1.8/manual/Installation.html</t>
+  </si>
+  <si>
+    <t>Refactorisation du code</t>
+  </si>
+  <si>
+    <t>Rédaction de la saisie du joueur</t>
+  </si>
+  <si>
+    <t>Rédaction du mouvement des pièces</t>
   </si>
 </sst>
 </file>
@@ -330,7 +351,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="169" formatCode="[h]:mm"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -451,6 +472,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -460,7 +482,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1212,19 +1233,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.38297872340425532</c:v>
+                  <c:v>0.45685279187817246</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31347517730496466</c:v>
+                  <c:v>0.43993231810490707</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.24539007092198595</c:v>
+                  <c:v>3.3840947546531303E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.8156028368794292E-2</c:v>
+                  <c:v>6.9373942470389111E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2238,8 +2259,8 @@
   </sheetPr>
   <dimension ref="B1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2257,16 +2278,16 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
@@ -3682,7 +3703,7 @@
       </c>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B64" s="8">
         <v>45429</v>
       </c>
@@ -3701,6 +3722,9 @@
       </c>
       <c r="G64" s="2" t="s">
         <v>91</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="J64" s="1"/>
     </row>
@@ -3727,44 +3751,135 @@
       <c r="J65" s="1"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E66" s="9"/>
+      <c r="B66" s="8">
+        <v>45433</v>
+      </c>
+      <c r="C66" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D66" s="9">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="E66" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67" s="8">
+        <v>45433</v>
+      </c>
+      <c r="C67" s="9">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="D67" s="9">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="E67" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B68" s="8">
+        <v>45433</v>
+      </c>
+      <c r="C68" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D68" s="9">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="E68" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69" s="8">
+        <v>45433</v>
+      </c>
+      <c r="C69" s="9">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D69" s="9">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="E69" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="J69" s="1"/>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70" s="8">
+        <v>45433</v>
+      </c>
+      <c r="C70" s="9">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D70" s="9">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E70" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="J70" s="1"/>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" s="8"/>
-      <c r="C71" s="9"/>
+      <c r="B71" s="8">
+        <v>45433</v>
+      </c>
+      <c r="C71" s="9">
+        <v>0.5625</v>
+      </c>
       <c r="D71" s="9"/>
       <c r="E71" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>-0.5625</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="J71" s="1"/>
     </row>
@@ -4002,11 +4117,13 @@
     <hyperlink ref="I51" r:id="rId6" xr:uid="{AA195AD4-FC1E-47FD-97C8-F3CA670D3842}"/>
     <hyperlink ref="I62" r:id="rId7" xr:uid="{1AEE26CC-3B7E-41DE-8082-7FEEC292C50C}"/>
     <hyperlink ref="I61" r:id="rId8" xr:uid="{6042347D-2CA2-432B-8086-DE5C6BD87881}"/>
+    <hyperlink ref="I68" r:id="rId9" xr:uid="{183277D3-BF31-4C46-9091-3C29B8981F33}"/>
+    <hyperlink ref="I64" r:id="rId10" xr:uid="{26CA2638-C028-4584-81E1-34EE6FCF95DE}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId9"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId11"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4063,11 +4180,11 @@
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>0.76736111111111094</v>
+        <v>0.90277777777777768</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>0.60069444444444442</v>
+        <v>6.944444444444442E-2</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -4077,9 +4194,9 @@
         <f>SUMIF(Tableau1[Sujet], Sheet1!H$3, Tableau1[Durée])</f>
         <v>0.14236111111111094</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="11">
         <f>SUM(D4:H4)</f>
-        <v>2.4479166666666652</v>
+        <v>2.0520833333333326</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -4088,15 +4205,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.38297872340425532</v>
+        <v>0.45685279187817246</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.31347517730496466</v>
+        <v>0.43993231810490707</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.24539007092198595</v>
+        <v>3.3840947546531303E-2</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -4104,11 +4221,11 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>5.8156028368794292E-2</v>
+        <v>6.9373942470389111E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>
-        <v>1.0000000000000002</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Rectification du mouvement des pièces
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F51373-BD0C-40FD-BC2F-B7F76E5C78D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF822FC0-47C7-488C-B1A6-EC0CC305FBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="104">
   <si>
     <t>Date</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>Rédaction du mouvement des pièces</t>
+  </si>
+  <si>
+    <t>Implémentation de la prévision du déplacement des pièces</t>
+  </si>
+  <si>
+    <t>Rédaction de la génération des mouvements des pièces</t>
   </si>
 </sst>
 </file>
@@ -1233,19 +1239,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.45685279187817246</c:v>
+                  <c:v>0.34659820282413345</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43993231810490707</c:v>
+                  <c:v>0.34146341463414642</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3840947546531303E-2</c:v>
+                  <c:v>0.25930680359435182</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.9373942470389111E-2</c:v>
+                  <c:v>5.2631578947368383E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2260,7 +2266,7 @@
   <dimension ref="B1:J106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3870,10 +3876,12 @@
       <c r="C71" s="9">
         <v>0.5625</v>
       </c>
-      <c r="D71" s="9"/>
+      <c r="D71" s="9">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="E71" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>-0.5625</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>2</v>
@@ -3884,24 +3892,68 @@
       <c r="J71" s="1"/>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" s="8"/>
+      <c r="B72" s="8">
+        <v>45433</v>
+      </c>
+      <c r="C72" s="9">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D72" s="9">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="E72" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J72" s="1"/>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B73" s="8">
+        <v>45433</v>
+      </c>
+      <c r="C73" s="9">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D73" s="9">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="E73" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="J73" s="1"/>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B74" s="8">
+        <v>45433</v>
+      </c>
+      <c r="C74" s="9">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D74" s="9">
+        <v>0.66319444444444442</v>
+      </c>
       <c r="E74" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.4305555555555469E-2</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="J74" s="1"/>
     </row>
@@ -4180,11 +4232,11 @@
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>0.90277777777777768</v>
+        <v>0.92361111111111094</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>6.944444444444442E-2</v>
+        <v>0.70138888888888884</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -4196,7 +4248,7 @@
       </c>
       <c r="I4" s="11">
         <f>SUM(D4:H4)</f>
-        <v>2.0520833333333326</v>
+        <v>2.7048611111111098</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -4205,15 +4257,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.45685279187817246</v>
+        <v>0.34659820282413345</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.43993231810490707</v>
+        <v>0.34146341463414642</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>3.3840947546531303E-2</v>
+        <v>0.25930680359435182</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -4221,11 +4273,11 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>6.9373942470389111E-2</v>
+        <v>5.2631578947368383E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Résolution d'erreur de la génération du mouvement des pièces
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF822FC0-47C7-488C-B1A6-EC0CC305FBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522569A4-73A0-4AF2-9D1C-C0A6565AB664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="106">
   <si>
     <t>Date</t>
   </si>
@@ -349,6 +349,12 @@
   </si>
   <si>
     <t>Rédaction de la génération des mouvements des pièces</t>
+  </si>
+  <si>
+    <t>Rectification du déplacement des pièces</t>
+  </si>
+  <si>
+    <t>Problème du script qui ne garde pas en mémoire les variable de la pièce, qui cause problème dans certain cas</t>
   </si>
 </sst>
 </file>
@@ -786,8 +792,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val -182261"/>
-                        <a:gd name="adj2" fmla="val -43804"/>
+                        <a:gd name="adj1" fmla="val -139066"/>
+                        <a:gd name="adj2" fmla="val 72204"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -962,8 +968,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 125081"/>
-                        <a:gd name="adj2" fmla="val 44709"/>
+                        <a:gd name="adj1" fmla="val 123904"/>
+                        <a:gd name="adj2" fmla="val 101225"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -1050,8 +1056,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 178795"/>
-                        <a:gd name="adj2" fmla="val 166624"/>
+                        <a:gd name="adj1" fmla="val 160912"/>
+                        <a:gd name="adj2" fmla="val 187446"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -1138,8 +1144,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 4602"/>
-                        <a:gd name="adj2" fmla="val 168600"/>
+                        <a:gd name="adj1" fmla="val -10206"/>
+                        <a:gd name="adj2" fmla="val 135880"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:noFill/>
@@ -1239,19 +1245,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.34659820282413345</c:v>
+                  <c:v>0.38848920863309339</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34146341463414642</c:v>
+                  <c:v>0.26187050359712238</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25930680359435182</c:v>
+                  <c:v>0.29064748201438856</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2631578947368383E-2</c:v>
+                  <c:v>5.899280575539563E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1889,8 +1895,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2265,8 +2271,8 @@
   </sheetPr>
   <dimension ref="B1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3957,17 +3963,44 @@
       </c>
       <c r="J74" s="1"/>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B75" s="8">
+        <v>45433</v>
+      </c>
+      <c r="C75" s="9">
+        <v>0.66319444444444442</v>
+      </c>
+      <c r="D75" s="9">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="E75" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="J75" s="1"/>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B76" s="8">
+        <v>45435</v>
+      </c>
+      <c r="C76" s="9">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="E76" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="J76" s="1"/>
     </row>
@@ -4188,7 +4221,7 @@
   <dimension ref="C3:I80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4232,7 +4265,7 @@
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>0.92361111111111094</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
@@ -4248,7 +4281,7 @@
       </c>
       <c r="I4" s="11">
         <f>SUM(D4:H4)</f>
-        <v>2.7048611111111098</v>
+        <v>2.4131944444444438</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -4257,15 +4290,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.34659820282413345</v>
+        <v>0.38848920863309339</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.34146341463414642</v>
+        <v>0.26187050359712238</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.25930680359435182</v>
+        <v>0.29064748201438856</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -4273,7 +4306,7 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>5.2631578947368383E-2</v>
+        <v>5.899280575539563E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>

</xml_diff>

<commit_message>
Implémentation de la génération du mouvement des pièces restantes
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522569A4-73A0-4AF2-9D1C-C0A6565AB664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A28ACC-6BA5-4C63-8DD8-FDF00CC05B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>Problème du script qui ne garde pas en mémoire les variable de la pièce, qui cause problème dans certain cas</t>
+  </si>
+  <si>
+    <t>Résolution d'erreur de la génération des mouvements des pièces</t>
+  </si>
+  <si>
+    <t>Implémentation de la génération du mouvement des pièces restante</t>
   </si>
 </sst>
 </file>
@@ -1245,19 +1251,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.38848920863309339</c:v>
+                  <c:v>0.33415841584158407</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26187050359712238</c:v>
+                  <c:v>0.36509900990099015</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29064748201438856</c:v>
+                  <c:v>0.25000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.899280575539563E-2</c:v>
+                  <c:v>5.0742574257425697E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2271,8 +2277,8 @@
   </sheetPr>
   <dimension ref="B1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G79" sqref="G78:G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,28 +3999,55 @@
         <v>45435</v>
       </c>
       <c r="C76" s="9">
-        <v>0.33333333333333331</v>
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D76" s="9">
+        <v>0.39930555555555558</v>
       </c>
       <c r="E76" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>-0.33333333333333331</v>
+        <v>3.125E-2</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G76" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="J76" s="1"/>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B77" s="8">
+        <v>45435</v>
+      </c>
+      <c r="C77" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D77" s="9">
+        <v>0.4375</v>
+      </c>
       <c r="E77" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="J77" s="1"/>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B78" s="8">
+        <v>45435</v>
+      </c>
+      <c r="C78" s="9">
+        <v>0.4375</v>
+      </c>
       <c r="E78" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>-0.4375</v>
       </c>
       <c r="J78" s="1"/>
     </row>
@@ -4265,7 +4298,7 @@
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>0.63194444444444442</v>
+        <v>1.0243055555555554</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
@@ -4281,7 +4314,7 @@
       </c>
       <c r="I4" s="11">
         <f>SUM(D4:H4)</f>
-        <v>2.4131944444444438</v>
+        <v>2.8055555555555545</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -4290,15 +4323,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.38848920863309339</v>
+        <v>0.33415841584158407</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.26187050359712238</v>
+        <v>0.36509900990099015</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.29064748201438856</v>
+        <v>0.25000000000000006</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -4306,7 +4339,7 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>5.899280575539563E-2</v>
+        <v>5.0742574257425697E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>

</xml_diff>

<commit_message>
Implémentation des méthodes de validation des coups
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A28ACC-6BA5-4C63-8DD8-FDF00CC05B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3B32A6-D00D-4B1D-B37B-83E556573FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -361,6 +361,15 @@
   </si>
   <si>
     <t>Implémentation de la génération du mouvement des pièces restante</t>
+  </si>
+  <si>
+    <t>Implémentation de la gestion de tour</t>
+  </si>
+  <si>
+    <t>Implémentation de la simulation d'une position pour faire la validation des mouvements d'une pièce</t>
+  </si>
+  <si>
+    <t>Implémentation de la validation d'une position</t>
   </si>
 </sst>
 </file>
@@ -1251,19 +1260,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.33415841584158407</c:v>
+                  <c:v>0.31505250875145846</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36509900990099015</c:v>
+                  <c:v>0.40140023337222869</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25000000000000006</c:v>
+                  <c:v>0.235705950991832</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0742574257425697E-2</c:v>
+                  <c:v>4.7841306884480697E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2278,7 +2287,7 @@
   <dimension ref="B1:J106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G79" sqref="G78:G79"/>
+      <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4045,117 +4054,171 @@
       <c r="C78" s="9">
         <v>0.4375</v>
       </c>
+      <c r="D78" s="9">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="E78" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>-0.4375</v>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="J78" s="1"/>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B79" s="8">
+        <v>45435</v>
+      </c>
+      <c r="C79" s="9">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D79" s="9">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E79" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B80" s="8">
+        <v>45435</v>
+      </c>
+      <c r="C80" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="D80" s="9">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E80" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="8">
+        <v>45435</v>
+      </c>
+      <c r="C81" s="9">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D81" s="9">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="E81" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>3.1249999999999889E-2</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="8"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
-      <c r="J79" s="1"/>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E80" s="9">
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E83" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
-      <c r="J80" s="1"/>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" s="9">
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E84" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="9">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E85" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="9">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E86" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="9">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E87" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E85" s="9">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E88" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E86" s="9">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E89" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E87" s="9">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E90" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E88" s="9">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E91" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E89" s="9">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E92" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E90" s="9">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E93" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E91" s="9">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E94" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E92" s="9">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E95" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E93" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E94" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E95" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E96" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
@@ -4254,7 +4317,7 @@
   <dimension ref="C3:I80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4298,7 +4361,7 @@
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>1.0243055555555554</v>
+        <v>1.1944444444444442</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
@@ -4314,7 +4377,7 @@
       </c>
       <c r="I4" s="11">
         <f>SUM(D4:H4)</f>
-        <v>2.8055555555555545</v>
+        <v>2.9756944444444438</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -4323,15 +4386,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.33415841584158407</v>
+        <v>0.31505250875145846</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.36509900990099015</v>
+        <v>0.40140023337222869</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.25000000000000006</v>
+        <v>0.235705950991832</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -4339,11 +4402,11 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>5.0742574257425697E-2</v>
+        <v>4.7841306884480697E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajout de la promotion des pièces et rectification du roque.
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6021ECAB-48EA-486F-A868-8062B8958ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F502E709-AAF9-42FD-8E2B-AD942E20E04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="119">
   <si>
     <t>Date</t>
   </si>
@@ -384,10 +384,16 @@
     <t>Résolution d'erreur pour le coup en passant</t>
   </si>
   <si>
-    <t>Implémentatoin du roque</t>
-  </si>
-  <si>
     <t>Résolution d'erreur du roque</t>
+  </si>
+  <si>
+    <t>Implémentation du roque</t>
+  </si>
+  <si>
+    <t>Implémentation de la promotion</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/64810646/delete-gameobject-before-the-end-of-the-frame</t>
   </si>
 </sst>
 </file>
@@ -1278,19 +1284,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.2863202545068928</c:v>
+                  <c:v>0.28066528066528057</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.45599151643690361</c:v>
+                  <c:v>0.46673596673596685</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21420996818663846</c:v>
+                  <c:v>0.20997920997921002</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3478260869565181E-2</c:v>
+                  <c:v>4.261954261954258E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2304,8 +2310,8 @@
   </sheetPr>
   <dimension ref="B1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4131,7 +4137,7 @@
       </c>
       <c r="J80" s="1"/>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="8">
         <v>45435</v>
       </c>
@@ -4152,7 +4158,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="8">
         <v>45436</v>
       </c>
@@ -4173,7 +4179,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="8">
         <v>45436</v>
       </c>
@@ -4194,7 +4200,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="8">
         <v>45436</v>
       </c>
@@ -4215,7 +4221,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="8">
         <v>45436</v>
       </c>
@@ -4236,7 +4242,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="8">
         <v>45436</v>
       </c>
@@ -4254,10 +4260,10 @@
         <v>4</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="8">
         <v>45436</v>
       </c>
@@ -4275,10 +4281,10 @@
         <v>4</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="8">
         <v>45436</v>
       </c>
@@ -4296,52 +4302,70 @@
         <v>4</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B89" s="8">
+        <v>45439</v>
+      </c>
+      <c r="C89" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="D89" s="9">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="E89" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E90" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E90" s="9">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E91" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E91" s="9">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E92" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E92" s="9">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E93" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E93" s="9">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E94" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E94" s="9">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E95" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E95" s="9">
-        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E96" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
         <v>0</v>
@@ -4423,11 +4447,12 @@
     <hyperlink ref="I61" r:id="rId8" xr:uid="{6042347D-2CA2-432B-8086-DE5C6BD87881}"/>
     <hyperlink ref="I68" r:id="rId9" xr:uid="{183277D3-BF31-4C46-9091-3C29B8981F33}"/>
     <hyperlink ref="I64" r:id="rId10" xr:uid="{26CA2638-C028-4584-81E1-34EE6FCF95DE}"/>
+    <hyperlink ref="I89" r:id="rId11" xr:uid="{528655AB-D797-445A-967B-97E2C7331F95}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId11"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4440,7 +4465,7 @@
   <dimension ref="C3:I80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4484,7 +4509,7 @@
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>1.4930555555555554</v>
+        <v>1.5590277777777777</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
@@ -4500,7 +4525,7 @@
       </c>
       <c r="I4" s="11">
         <f>SUM(D4:H4)</f>
-        <v>3.2743055555555545</v>
+        <v>3.3402777777777768</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -4509,15 +4534,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.2863202545068928</v>
+        <v>0.28066528066528057</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.45599151643690361</v>
+        <v>0.46673596673596685</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.21420996818663846</v>
+        <v>0.20997920997921002</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -4525,7 +4550,7 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>4.3478260869565181E-2</v>
+        <v>4.261954261954258E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>

</xml_diff>

<commit_message>
Modification du menu pour lancer le jeu
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F502E709-AAF9-42FD-8E2B-AD942E20E04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEEB09A-4B84-42CB-8559-B7906B7EA0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="121">
   <si>
     <t>Date</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/64810646/delete-gameobject-before-the-end-of-the-frame</t>
+  </si>
+  <si>
+    <t>https://docs.unity3d.com/ScriptReference/SceneManagement.SceneManager.LoadScene.html</t>
+  </si>
+  <si>
+    <t>Modification du menu pour le jeu et réalisation du build du jeu</t>
   </si>
 </sst>
 </file>
@@ -1284,19 +1290,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.28066528066528057</c:v>
+                  <c:v>0.31177829099307147</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46673596673596685</c:v>
+                  <c:v>0.40762124711316405</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20997920997921002</c:v>
+                  <c:v>0.23325635103926101</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.261954261954258E-2</c:v>
+                  <c:v>4.7344110854503414E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2310,8 +2316,8 @@
   </sheetPr>
   <dimension ref="B1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I90" sqref="I90"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4329,10 +4335,25 @@
         <v>118</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B90" s="8">
+        <v>45440</v>
+      </c>
+      <c r="C90" s="9">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="E90" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
@@ -4448,11 +4469,12 @@
     <hyperlink ref="I68" r:id="rId9" xr:uid="{183277D3-BF31-4C46-9091-3C29B8981F33}"/>
     <hyperlink ref="I64" r:id="rId10" xr:uid="{26CA2638-C028-4584-81E1-34EE6FCF95DE}"/>
     <hyperlink ref="I89" r:id="rId11" xr:uid="{528655AB-D797-445A-967B-97E2C7331F95}"/>
+    <hyperlink ref="I90" r:id="rId12" xr:uid="{DBEBDA19-40E6-4508-9A35-4BA1CC05A74D}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId12"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4509,7 +4531,7 @@
       </c>
       <c r="E4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!E$3, Tableau1[Durée])</f>
-        <v>1.5590277777777777</v>
+        <v>1.2256944444444444</v>
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
@@ -4525,7 +4547,7 @@
       </c>
       <c r="I4" s="11">
         <f>SUM(D4:H4)</f>
-        <v>3.3402777777777768</v>
+        <v>3.0069444444444438</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -4534,15 +4556,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.28066528066528057</v>
+        <v>0.31177829099307147</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.46673596673596685</v>
+        <v>0.40762124711316405</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.20997920997921002</v>
+        <v>0.23325635103926101</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -4550,11 +4572,11 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>4.261954261954258E-2</v>
+        <v>4.7344110854503414E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mise à jour final de la documentation
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt05klk\Desktop\DossierTPI\Jeu_dechec_sur_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320950C9-4052-496D-9D97-3518EBF0058E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B969E4-0F1A-4A9C-AF01-C9FC356C1BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C5A27D1-6DF5-49AD-8CFF-A09824726FDF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="141">
   <si>
     <t>Date</t>
   </si>
@@ -445,6 +445,21 @@
   </si>
   <si>
     <t>Rédaction des conditions de fin de partie</t>
+  </si>
+  <si>
+    <t>Rédaction de la conclusion</t>
+  </si>
+  <si>
+    <t>Rédaction du résumé</t>
+  </si>
+  <si>
+    <t>Rédaction des sources, le manuel d'installation et d'utilisation</t>
+  </si>
+  <si>
+    <t>Création et rédaction de la planification final</t>
+  </si>
+  <si>
+    <t>Impression et envoi du TPI</t>
   </si>
 </sst>
 </file>
@@ -1335,19 +1350,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.25886864813039301</c:v>
+                  <c:v>0.24907749077490765</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43432406519654848</c:v>
+                  <c:v>0.41789667896678973</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.26749760306807285</c:v>
+                  <c:v>0.29243542435424352</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9309683604985581E-2</c:v>
+                  <c:v>4.0590405904058997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2015,8 +2030,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}" name="Tableau1" displayName="Tableau1" ref="B3:I106" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="B3:I106" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}" name="Tableau1" displayName="Tableau1" ref="B3:I110" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="B3:I110" xr:uid="{C725EC7A-009E-4CEC-9940-8C10EB632C97}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{799BD6A8-A92C-43CC-B95D-FF1653CA16C4}" name="Date" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{1380C259-FA2D-4EA6-91E9-BF1969E7CC18}" name="Début" dataDxfId="6"/>
@@ -2359,10 +2374,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J106"/>
+  <dimension ref="B1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4702,17 +4717,129 @@
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="8"/>
-      <c r="C105" s="9"/>
+      <c r="B105" s="8">
+        <v>45442</v>
+      </c>
+      <c r="C105" s="9">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D105" s="9">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="E105" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="8">
+        <v>45442</v>
+      </c>
+      <c r="C106" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D106" s="9">
+        <v>0.43402777777777773</v>
+      </c>
       <c r="E106" s="9">
         <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.4305555555555469E-2</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B107" s="8">
+        <v>45442</v>
+      </c>
+      <c r="C107" s="9">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="D107" s="9">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="E107" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B108" s="8">
+        <v>45442</v>
+      </c>
+      <c r="C108" s="9">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D108" s="9">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E108" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B109" s="8">
+        <v>45442</v>
+      </c>
+      <c r="C109" s="9">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D109" s="9">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E109" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B110" s="8">
+        <v>45442</v>
+      </c>
+      <c r="C110" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="D110" s="9">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E110" s="9">
+        <f>Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]]</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4750,7 +4877,7 @@
   <dimension ref="C3:I80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="B3" sqref="B3:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4798,7 +4925,7 @@
       </c>
       <c r="F4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!F$3, Tableau1[Durée])</f>
-        <v>0.96874999999999978</v>
+        <v>1.1006944444444442</v>
       </c>
       <c r="G4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!G$3, Tableau1[Durée])</f>
@@ -4806,11 +4933,11 @@
       </c>
       <c r="H4" s="4">
         <f>SUMIF(Tableau1[Sujet], Sheet1!H$3, Tableau1[Durée])</f>
-        <v>0.14236111111111094</v>
+        <v>0.15277777777777757</v>
       </c>
       <c r="I4" s="11">
         <f>SUM(D4:H4)</f>
-        <v>3.6215277777777768</v>
+        <v>3.763888888888888</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -4819,15 +4946,15 @@
       </c>
       <c r="D5" s="6">
         <f>D4/$I$4</f>
-        <v>0.25886864813039301</v>
+        <v>0.24907749077490765</v>
       </c>
       <c r="E5" s="6">
         <f>E4/$I$4</f>
-        <v>0.43432406519654848</v>
+        <v>0.41789667896678973</v>
       </c>
       <c r="F5" s="6">
         <f>F4/$I$4</f>
-        <v>0.26749760306807285</v>
+        <v>0.29243542435424352</v>
       </c>
       <c r="G5" s="6">
         <f>G4/$I$4</f>
@@ -4835,11 +4962,11 @@
       </c>
       <c r="H5" s="6">
         <f>H4/$I$4</f>
-        <v>3.9309683604985581E-2</v>
+        <v>4.0590405904058997E-2</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Table2[[#This Row],[Analyse]:[Autres]])</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>